<commit_message>
thematic ,non-quantative,quantatitive Attribute and classiffication is fiished
</commit_message>
<xml_diff>
--- a/test/xlsx_random_tree_dataset_1.xlsx
+++ b/test/xlsx_random_tree_dataset_1.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27531"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27628"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Shubham\Desktop\Data-Quality\Data-Quality\test files\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Shubham\Desktop\bisag\Data-Quality\Data-Quality\test\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E36F8E4-E09B-4CCC-A496-83A815082E4C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1DC45484-18DB-45D2-B4D0-CF195390250C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -388,7 +388,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -405,6 +405,9 @@
     <xf numFmtId="17" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -722,7 +725,7 @@
   <dimension ref="A1:H51"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H22" sqref="H22"/>
+      <selection activeCell="H3" sqref="H3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -780,7 +783,7 @@
       <c r="G2" s="3">
         <v>40980</v>
       </c>
-      <c r="H2" s="3">
+      <c r="H2" s="12">
         <v>43173</v>
       </c>
     </row>
@@ -806,7 +809,7 @@
       <c r="G3" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="H3" s="1" t="s">
+      <c r="H3" s="12" t="s">
         <v>21</v>
       </c>
     </row>
@@ -986,7 +989,7 @@
       <c r="G10" s="9">
         <v>40972</v>
       </c>
-      <c r="H10" s="9">
+      <c r="H10" s="11">
         <v>40982</v>
       </c>
     </row>

</xml_diff>